<commit_message>
Se agrega al modelo los partidos y sus respectivas estadisticas.
</commit_message>
<xml_diff>
--- a/src/main/java/application/excel/QAC.xlsx
+++ b/src/main/java/application/excel/QAC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://cdnmd.lavoz.com.ar/sites/default/files/styles/width_1072/public/nota_periodistica/chapu-brana-quilmes.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claudio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bieler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1989-11-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.estadio.ec/sites/default/files/fotos/2017/01/06/bieler_crop1442507746687.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebastian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1979-11-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://elsolnoticias.com.ar/wp-content/uploads/2018/01/SCR.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre Equipo</t>
@@ -209,15 +233,13 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="67.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="66.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,6 +320,46 @@
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>19345677</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>19345677</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -306,6 +368,8 @@
     <hyperlink ref="F2" r:id="rId1" display="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSl0xmQdlV9AIhAd-4qmz5hGypf6YrM8406xAycltu9rqB2uiYgLw"/>
     <hyperlink ref="F3" r:id="rId2" display="http://www.laprensa.com.ar/multimedios/imgs/54533_620.JPG"/>
     <hyperlink ref="F4" r:id="rId3" display="https://cdnmd.lavoz.com.ar/sites/default/files/styles/width_1072/public/nota_periodistica/chapu-brana-quilmes.jpg"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://www.estadio.ec/sites/default/files/fotos/2017/01/06/bieler_crop1442507746687.jpg"/>
+    <hyperlink ref="F6" r:id="rId5" display="http://elsolnoticias.com.ar/wp-content/uploads/2018/01/SCR.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -330,19 +394,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1"/>
     </row>

</xml_diff>